<commit_message>
Replace SoCDTtiNTY values with 1 divided by AVL values
</commit_message>
<xml_diff>
--- a/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
+++ b/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
@@ -5,24 +5,40 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\South Korea\eps-southkorea\InputData\trans\SoCDTtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\trans\SoCDTtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA43F75-04C3-4360-BF30-E907E8C607F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553FCB52-91FB-46F5-B3ED-F82C34C79BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10620" yWindow="210" windowWidth="14570" windowHeight="13590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="SoCDTtiNTY-psgr" sheetId="2" r:id="rId2"/>
-    <sheet name="SoCDTtiNTY-frgt" sheetId="4" r:id="rId3"/>
+    <sheet name="AVL" sheetId="5" r:id="rId2"/>
+    <sheet name="SoCDTtiNTY-psgr" sheetId="2" r:id="rId3"/>
+    <sheet name="SoCDTtiNTY-frgt" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>SoCDTtiNTY Share of Cargo Dist Transported that is New This Year</t>
   </si>
@@ -100,12 +116,27 @@
   </si>
   <si>
     <t>hydrogen vehicle</t>
+  </si>
+  <si>
+    <t>Vehicle Lifetime (years)</t>
+  </si>
+  <si>
+    <t>Passenger</t>
+  </si>
+  <si>
+    <t>Freight</t>
+  </si>
+  <si>
+    <t>Calculated SoCDTtiNTY values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -143,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -155,6 +186,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -170,6 +206,59 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="About"/>
+      <sheetName val="NTS 1-20"/>
+      <sheetName val="Data"/>
+      <sheetName val="SK calcs"/>
+      <sheetName val="AVL"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="16">
+          <cell r="A16">
+            <v>24</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="C22">
+            <v>34</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28">
+            <v>33</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>17.22332068760786</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="23">
+          <cell r="D23">
+            <v>11.42095169122128</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="D29">
+            <v>13.396516093228287</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -495,16 +584,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -512,47 +601,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -563,23 +652,221 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE974D0-35AB-448C-ABAC-291E7575B7A2}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6">
+        <f>'[1]SK calcs'!D23</f>
+        <v>11.42095169122128</v>
+      </c>
+      <c r="C2" s="6">
+        <f t="shared" ref="C2:C7" si="0">B2</f>
+        <v>11.42095169122128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6">
+        <f>'[1]SK calcs'!D29</f>
+        <v>13.396516093228287</v>
+      </c>
+      <c r="C3" s="6">
+        <f t="shared" si="0"/>
+        <v>13.396516093228287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="6">
+        <f>ROUND([1]Data!A16,0)</f>
+        <v>24</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <f>ROUND([1]Data!C22,0)</f>
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <f>ROUND([1]Data!C28,0)</f>
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <f>ROUND([1]Data!A48,0)</f>
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7">
+        <f>1/B2</f>
+        <v>8.7558377535967555E-2</v>
+      </c>
+      <c r="C11" s="7">
+        <f>1/C2</f>
+        <v>8.7558377535967555E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="7">
+        <f t="shared" ref="B12:C16" si="1">1/B3</f>
+        <v>7.4646273183330336E-2</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="1"/>
+        <v>7.4646273183330336E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="7">
+        <f t="shared" si="1"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="1"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="7">
+        <f t="shared" si="1"/>
+        <v>2.9411764705882353E-2</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="1"/>
+        <v>2.9411764705882353E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="7">
+        <f t="shared" si="1"/>
+        <v>3.0303030303030304E-2</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="1"/>
+        <v>3.0303030303030304E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="7">
+        <f t="shared" si="1"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="1"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" customWidth="1"/>
-    <col min="2" max="8" width="14.36328125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -605,160 +892,202 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.36973314103415234</v>
+        <f>AVL!$B$11</f>
+        <v>8.7558377535967555E-2</v>
       </c>
       <c r="C2">
-        <v>7.1999999999999995E-2</v>
+        <f>AVL!$B$11</f>
+        <v>8.7558377535967555E-2</v>
       </c>
       <c r="D2">
+        <f>AVL!$B$11</f>
         <v>8.7558377535967555E-2</v>
       </c>
       <c r="E2">
-        <v>8.7558377535967569E-2</v>
+        <f>AVL!$B$11</f>
+        <v>8.7558377535967555E-2</v>
       </c>
       <c r="F2">
-        <v>7.1999999999999995E-2</v>
+        <f>AVL!$B$11</f>
+        <v>8.7558377535967555E-2</v>
       </c>
       <c r="G2">
-        <v>7.1999999999999995E-2</v>
+        <f>AVL!$B$11</f>
+        <v>8.7558377535967555E-2</v>
       </c>
       <c r="H2">
-        <v>0.82355077719697611</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <f>AVL!$B$11</f>
+        <v>8.7558377535967555E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
-        <v>0.95013940882091774</v>
+        <f>AVL!$B$12</f>
+        <v>7.4646273183330336E-2</v>
       </c>
       <c r="C3">
+        <f>AVL!$B$12</f>
         <v>7.4646273183330336E-2</v>
       </c>
       <c r="D3">
+        <f>AVL!$B$12</f>
         <v>7.4646273183330336E-2</v>
       </c>
       <c r="E3">
+        <f>AVL!$B$12</f>
         <v>7.4646273183330336E-2</v>
       </c>
       <c r="F3">
+        <f>AVL!$B$12</f>
         <v>7.4646273183330336E-2</v>
       </c>
       <c r="G3">
+        <f>AVL!$B$12</f>
         <v>7.4646273183330336E-2</v>
       </c>
       <c r="H3">
-        <v>7.4646273183330336E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <f>AVL!$B$12</f>
+        <v>7.4646273183330336E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
-        <v>0.08</v>
+        <f>AVL!$B$13</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C4">
-        <v>0.08</v>
+        <f>AVL!$B$13</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D4">
-        <v>0.08</v>
+        <f>AVL!$B$13</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="E4">
-        <v>0.08</v>
+        <f>AVL!$B$13</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="F4">
-        <v>0.08</v>
+        <f>AVL!$B$13</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="G4">
-        <v>0.08</v>
+        <f>AVL!$B$13</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="H4">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <f>AVL!$B$13</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5">
-        <v>2.9000000000000001E-2</v>
+        <f>AVL!$B$14</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="C5">
-        <v>2.9000000000000001E-2</v>
+        <f>AVL!$B$14</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="D5">
-        <v>2.9000000000000001E-2</v>
+        <f>AVL!$B$14</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="E5">
-        <v>2.9000000000000001E-2</v>
+        <f>AVL!$B$14</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="F5">
-        <v>2.9000000000000001E-2</v>
+        <f>AVL!$B$14</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="G5">
-        <v>2.9000000000000001E-2</v>
+        <f>AVL!$B$14</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="H5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <f>AVL!$B$14</f>
+        <v>2.9411764705882353E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6">
-        <v>2.9819999999999999E-2</v>
+        <f>AVL!$B$15</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="C6">
-        <v>2.9819999999999999E-2</v>
+        <f>AVL!$B$15</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="D6">
-        <v>2.9819999999999999E-2</v>
+        <f>AVL!$B$15</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="E6">
-        <v>2.9819999999999999E-2</v>
+        <f>AVL!$B$15</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="F6">
-        <v>2.9819999999999999E-2</v>
+        <f>AVL!$B$15</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="G6">
-        <v>2.9819999999999999E-2</v>
+        <f>AVL!$B$15</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="H6">
-        <v>2.9819999999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <f>AVL!$B$15</f>
+        <v>3.0303030303030304E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7">
-        <v>5.8700000000000002E-2</v>
+        <f>AVL!$B$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="C7">
-        <v>5.8700000000000002E-2</v>
+        <f>AVL!$B$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="D7">
-        <v>5.8000000000000003E-2</v>
+        <f>AVL!$B$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="E7">
-        <v>5.8700000000000002E-2</v>
+        <f>AVL!$B$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="F7">
-        <v>5.8700000000000002E-2</v>
+        <f>AVL!$B$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="G7">
-        <v>5.8700000000000002E-2</v>
+        <f>AVL!$B$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="H7">
-        <v>5.8700000000000002E-2</v>
+        <f>AVL!$B$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +1095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -774,16 +1103,16 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B7" sqref="B7:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" customWidth="1"/>
-    <col min="2" max="8" width="14.36328125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -809,160 +1138,202 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.36973314103415234</v>
+        <f>AVL!$C$11</f>
+        <v>8.7558377535967555E-2</v>
       </c>
       <c r="C2">
-        <v>7.1999999999999995E-2</v>
+        <f>AVL!$C$11</f>
+        <v>8.7558377535967555E-2</v>
       </c>
       <c r="D2">
+        <f>AVL!$C$11</f>
         <v>8.7558377535967555E-2</v>
       </c>
       <c r="E2">
-        <v>8.7558377535967569E-2</v>
+        <f>AVL!$C$11</f>
+        <v>8.7558377535967555E-2</v>
       </c>
       <c r="F2">
-        <v>7.1999999999999995E-2</v>
+        <f>AVL!$C$11</f>
+        <v>8.7558377535967555E-2</v>
       </c>
       <c r="G2">
-        <v>7.1999999999999995E-2</v>
+        <f>AVL!$C$11</f>
+        <v>8.7558377535967555E-2</v>
       </c>
       <c r="H2">
-        <v>0.82355077719697611</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <f>AVL!$C$11</f>
+        <v>8.7558377535967555E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
-        <v>0.95013940882091774</v>
+        <f>AVL!$C$12</f>
+        <v>7.4646273183330336E-2</v>
       </c>
       <c r="C3">
+        <f>AVL!$C$12</f>
         <v>7.4646273183330336E-2</v>
       </c>
       <c r="D3">
+        <f>AVL!$C$12</f>
         <v>7.4646273183330336E-2</v>
       </c>
       <c r="E3">
+        <f>AVL!$C$12</f>
         <v>7.4646273183330336E-2</v>
       </c>
       <c r="F3">
+        <f>AVL!$C$12</f>
         <v>7.4646273183330336E-2</v>
       </c>
       <c r="G3">
+        <f>AVL!$C$12</f>
         <v>7.4646273183330336E-2</v>
       </c>
       <c r="H3">
-        <v>7.4646273183330336E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <f>AVL!$C$12</f>
+        <v>7.4646273183330336E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
-        <v>0.08</v>
+        <f>AVL!$C$13</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C4">
-        <v>0.08</v>
+        <f>AVL!$C$13</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D4">
-        <v>0.08</v>
+        <f>AVL!$C$13</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="E4">
-        <v>0.08</v>
+        <f>AVL!$C$13</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="F4">
-        <v>0.08</v>
+        <f>AVL!$C$13</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="G4">
-        <v>0.08</v>
+        <f>AVL!$C$13</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="H4">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <f>AVL!$C$13</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5">
-        <v>2.9000000000000001E-2</v>
+        <f>AVL!$C$14</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="C5">
-        <v>2.9000000000000001E-2</v>
+        <f>AVL!$C$14</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="D5">
-        <v>2.9000000000000001E-2</v>
+        <f>AVL!$C$14</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="E5">
-        <v>2.9000000000000001E-2</v>
+        <f>AVL!$C$14</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="F5">
-        <v>2.9000000000000001E-2</v>
+        <f>AVL!$C$14</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="G5">
-        <v>2.9000000000000001E-2</v>
+        <f>AVL!$C$14</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="H5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <f>AVL!$C$14</f>
+        <v>2.9411764705882353E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6">
-        <v>3.0300000000000001E-2</v>
+        <f>AVL!$C$15</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="C6">
-        <v>3.0300000000000001E-2</v>
+        <f>AVL!$C$15</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="D6">
-        <v>3.0300000000000001E-2</v>
+        <f>AVL!$C$15</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="E6">
-        <v>3.0300000000000001E-2</v>
+        <f>AVL!$C$15</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="F6">
-        <v>3.0300000000000001E-2</v>
+        <f>AVL!$C$15</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="G6">
-        <v>3.0300000000000001E-2</v>
+        <f>AVL!$C$15</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="H6">
-        <v>3.0300000000000001E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <f>AVL!$C$15</f>
+        <v>3.0303030303030304E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7">
-        <v>0.06</v>
+        <f>AVL!$C$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="C7">
-        <v>0.06</v>
+        <f>AVL!$C$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="D7">
-        <v>0.06</v>
+        <f>AVL!$C$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="E7">
-        <v>0.06</v>
+        <f>AVL!$C$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="F7">
-        <v>0.06</v>
+        <f>AVL!$C$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="G7">
-        <v>0.06</v>
+        <f>AVL!$C$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="H7">
-        <v>0.06</v>
+        <f>AVL!$C$16</f>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>